<commit_message>
switched receipt and order columns
</commit_message>
<xml_diff>
--- a/Order Report to Sales Receipt column conversion.xlsx
+++ b/Order Report to Sales Receipt column conversion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sophiazhi/Documents/GitHub/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A28C75B9-07DB-2E4C-892F-119F4AC684D0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE3C9627-CD84-E746-AFB2-CC1847068F86}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1120" yWindow="1440" windowWidth="27240" windowHeight="15060" xr2:uid="{242A126C-CB64-D641-BBDC-20517CD8CB4E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="131">
   <si>
     <t>Order ID</t>
   </si>
@@ -351,9 +351,6 @@
     <t>Custom Sales Receipt</t>
   </si>
   <si>
-    <t>original (store order report) column</t>
-  </si>
-  <si>
     <t>sales receipt column</t>
   </si>
   <si>
@@ -399,244 +396,28 @@
     <t>N</t>
   </si>
   <si>
-    <t>P</t>
-  </si>
-  <si>
-    <t>Q</t>
-  </si>
-  <si>
     <t>R</t>
   </si>
   <si>
-    <t>S</t>
-  </si>
-  <si>
-    <t>T</t>
-  </si>
-  <si>
-    <t>O</t>
-  </si>
-  <si>
-    <t>U</t>
-  </si>
-  <si>
-    <t>V</t>
-  </si>
-  <si>
-    <t>W</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>Z</t>
-  </si>
-  <si>
-    <t>AA</t>
-  </si>
-  <si>
-    <t>AB</t>
-  </si>
-  <si>
-    <t>AC</t>
-  </si>
-  <si>
-    <t>AD</t>
-  </si>
-  <si>
-    <t>AE</t>
-  </si>
-  <si>
-    <t>AF</t>
-  </si>
-  <si>
-    <t>AG</t>
-  </si>
-  <si>
-    <t>AH</t>
-  </si>
-  <si>
-    <t>AI</t>
-  </si>
-  <si>
-    <t>AJ</t>
-  </si>
-  <si>
-    <t>AK</t>
-  </si>
-  <si>
-    <t>AL</t>
-  </si>
-  <si>
-    <t>AM</t>
-  </si>
-  <si>
-    <t>AN</t>
-  </si>
-  <si>
-    <t>AO</t>
-  </si>
-  <si>
-    <t>AP</t>
-  </si>
-  <si>
-    <t>AQ</t>
-  </si>
-  <si>
-    <t>AR</t>
-  </si>
-  <si>
-    <t>AS</t>
-  </si>
-  <si>
-    <t>AT</t>
-  </si>
-  <si>
-    <t>AU</t>
-  </si>
-  <si>
-    <t>AV</t>
-  </si>
-  <si>
-    <t>AW</t>
-  </si>
-  <si>
-    <t>AX</t>
-  </si>
-  <si>
-    <t>AY</t>
-  </si>
-  <si>
-    <t>AZ</t>
-  </si>
-  <si>
-    <t>BA</t>
-  </si>
-  <si>
-    <t>BB</t>
-  </si>
-  <si>
     <t>BC</t>
   </si>
   <si>
     <t>BD</t>
   </si>
   <si>
-    <t>BE</t>
-  </si>
-  <si>
-    <t>BF</t>
-  </si>
-  <si>
-    <t>BG</t>
-  </si>
-  <si>
-    <t>BI</t>
-  </si>
-  <si>
-    <t>BJ</t>
-  </si>
-  <si>
-    <t>BH</t>
-  </si>
-  <si>
-    <t>BK</t>
-  </si>
-  <si>
-    <t>BL</t>
-  </si>
-  <si>
-    <t>BM</t>
-  </si>
-  <si>
-    <t>BN</t>
-  </si>
-  <si>
-    <t>BO</t>
-  </si>
-  <si>
-    <t>BP</t>
-  </si>
-  <si>
-    <t>original content</t>
-  </si>
-  <si>
-    <t>order date</t>
-  </si>
-  <si>
-    <t>order ID</t>
-  </si>
-  <si>
-    <t>subtotal (incl tax)</t>
-  </si>
-  <si>
-    <t>subtotal (ex tax)</t>
-  </si>
-  <si>
-    <t>tax total</t>
-  </si>
-  <si>
-    <t>shipping cost (incl tax)</t>
-  </si>
-  <si>
-    <t>shipping cost (ex tax)</t>
-  </si>
-  <si>
-    <t>handling cost (incl tax)</t>
-  </si>
-  <si>
-    <t>handling cost (ex tax)</t>
-  </si>
-  <si>
-    <t>order total (incl tax)</t>
-  </si>
-  <si>
-    <t>order total (ex tax)</t>
-  </si>
-  <si>
-    <t>customer ID</t>
-  </si>
-  <si>
-    <t>customer name</t>
-  </si>
-  <si>
-    <t>customer email</t>
-  </si>
-  <si>
-    <t>custoner phone</t>
-  </si>
-  <si>
-    <t>ship method</t>
-  </si>
-  <si>
-    <t>payment method</t>
-  </si>
-  <si>
-    <t>F?</t>
-  </si>
-  <si>
-    <t>order status</t>
-  </si>
-  <si>
-    <t>/</t>
-  </si>
-  <si>
-    <t>C?</t>
-  </si>
-  <si>
-    <t>/ or F?</t>
-  </si>
-  <si>
-    <t>product SKU</t>
-  </si>
-  <si>
     <t>column K in sales receipt is sum of column I for all items with the same value in F</t>
   </si>
   <si>
-    <t>product quantity</t>
+    <t>original (store order) column)</t>
+  </si>
+  <si>
+    <t>A or M</t>
+  </si>
+  <si>
+    <t>N?</t>
+  </si>
+  <si>
+    <t>sum of values in column I for all items with the same value in F</t>
   </si>
 </sst>
 </file>
@@ -1021,10 +802,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFAC7848-BF4A-FF46-BADD-91F35C99B85C}">
-  <dimension ref="A1:BP75"/>
+  <dimension ref="A1:BP22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1507,478 +1288,109 @@
         <v>107</v>
       </c>
     </row>
-    <row r="7" spans="1:68" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>108</v>
-      </c>
-      <c r="B7" t="s">
-        <v>178</v>
-      </c>
-      <c r="C7" t="s">
-        <v>109</v>
-      </c>
-    </row>
     <row r="8" spans="1:68" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B8" t="s">
-        <v>180</v>
-      </c>
-      <c r="C8" t="s">
-        <v>196</v>
+        <v>127</v>
       </c>
       <c r="F8" t="s">
-        <v>202</v>
+        <v>126</v>
       </c>
     </row>
     <row r="9" spans="1:68" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>111</v>
-      </c>
-      <c r="B9" t="s">
-        <v>197</v>
-      </c>
-      <c r="C9" t="s">
-        <v>198</v>
+        <v>109</v>
       </c>
     </row>
     <row r="10" spans="1:68" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B10" t="s">
-        <v>179</v>
-      </c>
-      <c r="C10" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="11" spans="1:68" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B11" t="s">
-        <v>181</v>
-      </c>
-      <c r="C11" t="s">
-        <v>198</v>
+        <v>129</v>
       </c>
     </row>
     <row r="12" spans="1:68" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>114</v>
-      </c>
-      <c r="B12" t="s">
-        <v>182</v>
-      </c>
-      <c r="C12" t="s">
-        <v>198</v>
+        <v>112</v>
       </c>
     </row>
     <row r="13" spans="1:68" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B13" t="s">
-        <v>183</v>
-      </c>
-      <c r="C13" t="s">
-        <v>198</v>
+        <v>123</v>
       </c>
     </row>
     <row r="14" spans="1:68" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B14" t="s">
-        <v>184</v>
-      </c>
-      <c r="C14" t="s">
-        <v>198</v>
+        <v>128</v>
       </c>
     </row>
     <row r="15" spans="1:68" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B15" t="s">
-        <v>185</v>
-      </c>
-      <c r="C15" t="s">
-        <v>198</v>
+        <v>125</v>
       </c>
     </row>
     <row r="16" spans="1:68" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>116</v>
+      </c>
+      <c r="B16" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>117</v>
+      </c>
+      <c r="B17" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>118</v>
       </c>
-      <c r="B16" t="s">
-        <v>186</v>
-      </c>
-      <c r="C16" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>119</v>
       </c>
-      <c r="B17" t="s">
-        <v>187</v>
-      </c>
-      <c r="C17" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+      <c r="B19" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>120</v>
       </c>
-      <c r="B18" t="s">
-        <v>188</v>
-      </c>
-      <c r="C18" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>121</v>
       </c>
-      <c r="B19" t="s">
-        <v>189</v>
-      </c>
-      <c r="C19" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
         <v>122</v>
-      </c>
-      <c r="B20" t="s">
-        <v>190</v>
-      </c>
-      <c r="C20" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>123</v>
-      </c>
-      <c r="B21" t="s">
-        <v>191</v>
-      </c>
-      <c r="C21" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>129</v>
-      </c>
-      <c r="B22" t="s">
-        <v>192</v>
-      </c>
-      <c r="C22" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>124</v>
-      </c>
-      <c r="B23" t="s">
-        <v>193</v>
-      </c>
-      <c r="C23" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>125</v>
-      </c>
-      <c r="B24" t="s">
-        <v>194</v>
-      </c>
-      <c r="C24" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>126</v>
-      </c>
-      <c r="B25" t="s">
-        <v>195</v>
-      </c>
-      <c r="C25" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
-        <v>164</v>
-      </c>
-      <c r="B62" t="s">
-        <v>203</v>
-      </c>
-      <c r="C62" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
-        <v>165</v>
-      </c>
-      <c r="B63" t="s">
-        <v>201</v>
-      </c>
-      <c r="C63" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A68" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A70" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A71" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A72" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A73" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A74" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A75" t="s">
-        <v>177</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Order Report to Sales Receipt column conversion.xlsx
</commit_message>
<xml_diff>
--- a/Order Report to Sales Receipt column conversion.xlsx
+++ b/Order Report to Sales Receipt column conversion.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sophiazhi/Documents/GitHub/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Umarbek Nasimov\Desktop\Oldways\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE3C9627-CD84-E746-AFB2-CC1847068F86}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{8BA5916E-0C42-4C19-AE93-C88632D1BEDB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1120" yWindow="1440" windowWidth="27240" windowHeight="15060" xr2:uid="{242A126C-CB64-D641-BBDC-20517CD8CB4E}"/>
+    <workbookView xWindow="1122" yWindow="1440" windowWidth="27240" windowHeight="15060" xr2:uid="{242A126C-CB64-D641-BBDC-20517CD8CB4E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="135">
   <si>
     <t>Order ID</t>
   </si>
@@ -354,54 +354,15 @@
     <t>sales receipt column</t>
   </si>
   <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
     <t>C</t>
   </si>
   <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>E</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>G</t>
-  </si>
-  <si>
-    <t>H</t>
-  </si>
-  <si>
-    <t>I</t>
-  </si>
-  <si>
-    <t>J</t>
-  </si>
-  <si>
     <t>K</t>
   </si>
   <si>
-    <t>L</t>
-  </si>
-  <si>
-    <t>M</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
     <t>R</t>
   </si>
   <si>
-    <t>BC</t>
-  </si>
-  <si>
     <t>BD</t>
   </si>
   <si>
@@ -411,13 +372,64 @@
     <t>original (store order) column)</t>
   </si>
   <si>
-    <t>A or M</t>
-  </si>
-  <si>
     <t>N?</t>
   </si>
   <si>
     <t>sum of values in column I for all items with the same value in F</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A: Customer </t>
+  </si>
+  <si>
+    <t>B: Date</t>
+  </si>
+  <si>
+    <t>C: Ref No</t>
+  </si>
+  <si>
+    <t>D: Class</t>
+  </si>
+  <si>
+    <t>E: Payment method</t>
+  </si>
+  <si>
+    <t>F: Memo</t>
+  </si>
+  <si>
+    <t>A or M?</t>
+  </si>
+  <si>
+    <t>G: Item</t>
+  </si>
+  <si>
+    <t>H: Quantity</t>
+  </si>
+  <si>
+    <t>I: Amount</t>
+  </si>
+  <si>
+    <t>J: Amount of Sales Received</t>
+  </si>
+  <si>
+    <t>K: Amount of transaction</t>
+  </si>
+  <si>
+    <t>L: Amount deposited</t>
+  </si>
+  <si>
+    <t>M: Date deposited to ctc</t>
+  </si>
+  <si>
+    <t>N: Template name</t>
+  </si>
+  <si>
+    <t>Customer Sales Receipt</t>
+  </si>
+  <si>
+    <t>BC or S?</t>
   </si>
 </sst>
 </file>
@@ -427,7 +439,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -456,13 +468,31 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -477,7 +507,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
@@ -488,6 +518,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -804,13 +836,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFAC7848-BF4A-FF46-BADD-91F35C99B85C}">
   <dimension ref="A1:BP22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
+  <cols>
+    <col min="1" max="1" width="23.44921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.84765625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.6484375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:68" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:68" x14ac:dyDescent="0.6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1016,7 +1053,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:68" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:68" x14ac:dyDescent="0.6">
       <c r="A2" s="1">
         <v>5046</v>
       </c>
@@ -1208,7 +1245,7 @@
       </c>
       <c r="BP2" s="4"/>
     </row>
-    <row r="4" spans="1:68" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:68" x14ac:dyDescent="0.6">
       <c r="A4" s="5" t="s">
         <v>88</v>
       </c>
@@ -1252,7 +1289,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="1:68" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:68" x14ac:dyDescent="0.6">
       <c r="A5" s="7" t="s">
         <v>102</v>
       </c>
@@ -1288,109 +1325,127 @@
         <v>107</v>
       </c>
     </row>
-    <row r="8" spans="1:68" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:68" x14ac:dyDescent="0.6">
       <c r="A8" t="s">
         <v>108</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="F8" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="9" spans="1:68" x14ac:dyDescent="0.6">
+      <c r="A9" t="s">
+        <v>118</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="10" spans="1:68" x14ac:dyDescent="0.6">
+      <c r="A10" t="s">
+        <v>119</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="11" spans="1:68" x14ac:dyDescent="0.6">
+      <c r="A11" t="s">
+        <v>120</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="12" spans="1:68" x14ac:dyDescent="0.6">
+      <c r="A12" t="s">
+        <v>121</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="13" spans="1:68" x14ac:dyDescent="0.6">
+      <c r="A13" t="s">
+        <v>122</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="14" spans="1:68" x14ac:dyDescent="0.6">
+      <c r="A14" t="s">
+        <v>123</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="15" spans="1:68" x14ac:dyDescent="0.6">
+      <c r="A15" t="s">
+        <v>125</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="16" spans="1:68" x14ac:dyDescent="0.6">
+      <c r="A16" t="s">
+        <v>126</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A17" t="s">
         <v>127</v>
       </c>
-      <c r="F8" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="9" spans="1:68" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="10" spans="1:68" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="B17" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="B10" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="11" spans="1:68" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>111</v>
-      </c>
-      <c r="B11" t="s">
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A18" t="s">
+        <v>128</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A19" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="12" spans="1:68" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="13" spans="1:68" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>113</v>
-      </c>
-      <c r="B13" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="14" spans="1:68" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>114</v>
-      </c>
-      <c r="B14" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="15" spans="1:68" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>115</v>
-      </c>
-      <c r="B15" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="16" spans="1:68" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="B19" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="B16" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A20" t="s">
+        <v>130</v>
+      </c>
+      <c r="B20" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="B17" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>119</v>
-      </c>
-      <c r="B19" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A21" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+        <v>131</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.6">
       <c r="A22" t="s">
-        <v>122</v>
+        <v>132</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -1398,5 +1453,6 @@
     <hyperlink ref="R2" r:id="rId1" xr:uid="{A1147B43-7F48-3D4B-AB40-695A96E66784}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>